<commit_message>
Changes made to optimality and feasibility cuts
</commit_message>
<xml_diff>
--- a/MILP/model_output/TS_Subproblem_Solution.xlsx
+++ b/MILP/model_output/TS_Subproblem_Solution.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="225">
   <si>
     <t>origin_id</t>
   </si>
@@ -50,9 +50,6 @@
     <t>train_1_3_dMo_t19</t>
   </si>
   <si>
-    <t>train_1_3_dTu_t43</t>
-  </si>
-  <si>
     <t>train_1_5_dMo_t18</t>
   </si>
   <si>
@@ -77,78 +74,6 @@
     <t>train_5_1_dMo_t15</t>
   </si>
   <si>
-    <t>dwell_1_t19</t>
-  </si>
-  <si>
-    <t>dwell_1_t20</t>
-  </si>
-  <si>
-    <t>dwell_1_t21</t>
-  </si>
-  <si>
-    <t>dwell_1_t22</t>
-  </si>
-  <si>
-    <t>dwell_1_t23</t>
-  </si>
-  <si>
-    <t>dwell_1_t24</t>
-  </si>
-  <si>
-    <t>dwell_1_t25</t>
-  </si>
-  <si>
-    <t>dwell_1_t26</t>
-  </si>
-  <si>
-    <t>dwell_1_t27</t>
-  </si>
-  <si>
-    <t>dwell_1_t28</t>
-  </si>
-  <si>
-    <t>dwell_1_t29</t>
-  </si>
-  <si>
-    <t>dwell_1_t30</t>
-  </si>
-  <si>
-    <t>dwell_1_t31</t>
-  </si>
-  <si>
-    <t>dwell_1_t32</t>
-  </si>
-  <si>
-    <t>dwell_1_t33</t>
-  </si>
-  <si>
-    <t>dwell_1_t34</t>
-  </si>
-  <si>
-    <t>dwell_1_t35</t>
-  </si>
-  <si>
-    <t>dwell_1_t36</t>
-  </si>
-  <si>
-    <t>dwell_1_t37</t>
-  </si>
-  <si>
-    <t>dwell_1_t38</t>
-  </si>
-  <si>
-    <t>dwell_1_t39</t>
-  </si>
-  <si>
-    <t>dwell_1_t40</t>
-  </si>
-  <si>
-    <t>dwell_1_t41</t>
-  </si>
-  <si>
-    <t>dwell_1_t42</t>
-  </si>
-  <si>
     <t>dwell_2_t16</t>
   </si>
   <si>
@@ -377,9 +302,6 @@
     <t>exit_Aarau_Chiasso_t22</t>
   </si>
   <si>
-    <t>exit_Aarau_Chiasso_t46</t>
-  </si>
-  <si>
     <t>entry_Aarau_Visp_t18</t>
   </si>
   <si>
@@ -422,9 +344,6 @@
     <t>Node1_t19</t>
   </si>
   <si>
-    <t>Node1_t43</t>
-  </si>
-  <si>
     <t>Node1_t18</t>
   </si>
   <si>
@@ -449,310 +368,244 @@
     <t>Node5_t15</t>
   </si>
   <si>
-    <t>Node1_t20</t>
-  </si>
-  <si>
-    <t>Node1_t21</t>
-  </si>
-  <si>
-    <t>Node1_t22</t>
-  </si>
-  <si>
-    <t>Node1_t23</t>
-  </si>
-  <si>
-    <t>Node1_t24</t>
+    <t>Node2_t16</t>
+  </si>
+  <si>
+    <t>Node2_t17</t>
+  </si>
+  <si>
+    <t>Node2_t18</t>
+  </si>
+  <si>
+    <t>Node2_t19</t>
+  </si>
+  <si>
+    <t>Node2_t20</t>
+  </si>
+  <si>
+    <t>Node2_t21</t>
+  </si>
+  <si>
+    <t>Node2_t22</t>
+  </si>
+  <si>
+    <t>Node2_t23</t>
+  </si>
+  <si>
+    <t>Node2_t24</t>
+  </si>
+  <si>
+    <t>Node2_t25</t>
+  </si>
+  <si>
+    <t>Node2_t26</t>
+  </si>
+  <si>
+    <t>Node2_t27</t>
+  </si>
+  <si>
+    <t>Node2_t28</t>
+  </si>
+  <si>
+    <t>Node2_t29</t>
+  </si>
+  <si>
+    <t>Node2_t30</t>
+  </si>
+  <si>
+    <t>Node2_t31</t>
+  </si>
+  <si>
+    <t>Node2_t32</t>
+  </si>
+  <si>
+    <t>Node2_t33</t>
+  </si>
+  <si>
+    <t>Node2_t34</t>
+  </si>
+  <si>
+    <t>Node2_t35</t>
+  </si>
+  <si>
+    <t>Node2_t36</t>
+  </si>
+  <si>
+    <t>Node2_t37</t>
+  </si>
+  <si>
+    <t>Node2_t38</t>
+  </si>
+  <si>
+    <t>Node2_t39</t>
+  </si>
+  <si>
+    <t>Node2_t40</t>
+  </si>
+  <si>
+    <t>Node2_t41</t>
+  </si>
+  <si>
+    <t>Node2_t42</t>
+  </si>
+  <si>
+    <t>Node2_t43</t>
+  </si>
+  <si>
+    <t>Node2_t44</t>
+  </si>
+  <si>
+    <t>Node2_t45</t>
+  </si>
+  <si>
+    <t>Node2_t46</t>
+  </si>
+  <si>
+    <t>Node2_t47</t>
+  </si>
+  <si>
+    <t>Node2_t48</t>
+  </si>
+  <si>
+    <t>Node2_t49</t>
+  </si>
+  <si>
+    <t>Node2_t50</t>
+  </si>
+  <si>
+    <t>Node2_t51</t>
+  </si>
+  <si>
+    <t>Node2_t52</t>
+  </si>
+  <si>
+    <t>Node2_t53</t>
+  </si>
+  <si>
+    <t>Node2_t54</t>
+  </si>
+  <si>
+    <t>Node2_t55</t>
+  </si>
+  <si>
+    <t>Node2_t56</t>
+  </si>
+  <si>
+    <t>Node2_t57</t>
+  </si>
+  <si>
+    <t>Node2_t58</t>
+  </si>
+  <si>
+    <t>Node2_t59</t>
+  </si>
+  <si>
+    <t>Node3_t23</t>
+  </si>
+  <si>
+    <t>Node3_t24</t>
+  </si>
+  <si>
+    <t>Node3_t25</t>
+  </si>
+  <si>
+    <t>Node3_t26</t>
+  </si>
+  <si>
+    <t>Node3_t27</t>
+  </si>
+  <si>
+    <t>Node3_t28</t>
+  </si>
+  <si>
+    <t>Node3_t29</t>
+  </si>
+  <si>
+    <t>Node3_t30</t>
+  </si>
+  <si>
+    <t>Node3_t31</t>
+  </si>
+  <si>
+    <t>Node3_t32</t>
+  </si>
+  <si>
+    <t>Node3_t33</t>
+  </si>
+  <si>
+    <t>Node3_t34</t>
+  </si>
+  <si>
+    <t>Node3_t35</t>
+  </si>
+  <si>
+    <t>Node3_t36</t>
+  </si>
+  <si>
+    <t>Node3_t37</t>
+  </si>
+  <si>
+    <t>Node3_t38</t>
+  </si>
+  <si>
+    <t>Node3_t39</t>
+  </si>
+  <si>
+    <t>Node3_t40</t>
+  </si>
+  <si>
+    <t>Node3_t41</t>
+  </si>
+  <si>
+    <t>Node3_t42</t>
+  </si>
+  <si>
+    <t>Node3_t43</t>
+  </si>
+  <si>
+    <t>Node3_t44</t>
+  </si>
+  <si>
+    <t>Node3_t45</t>
+  </si>
+  <si>
+    <t>Node3_t64</t>
+  </si>
+  <si>
+    <t>Node3_t65</t>
+  </si>
+  <si>
+    <t>Node3_t66</t>
+  </si>
+  <si>
+    <t>Node3_t67</t>
+  </si>
+  <si>
+    <t>Node3_t68</t>
+  </si>
+  <si>
+    <t>Node3_t69</t>
+  </si>
+  <si>
+    <t>OD_Aarau_Chiasso_source</t>
+  </si>
+  <si>
+    <t>OD_Aarau_Visp_source</t>
+  </si>
+  <si>
+    <t>Node5_t22</t>
+  </si>
+  <si>
+    <t>OD_Baselwolf_Chiasso_source</t>
+  </si>
+  <si>
+    <t>Node3_t16</t>
+  </si>
+  <si>
+    <t>OD_Chiasso_Aarau_source</t>
   </si>
   <si>
     <t>Node1_t25</t>
-  </si>
-  <si>
-    <t>Node1_t26</t>
-  </si>
-  <si>
-    <t>Node1_t27</t>
-  </si>
-  <si>
-    <t>Node1_t28</t>
-  </si>
-  <si>
-    <t>Node1_t29</t>
-  </si>
-  <si>
-    <t>Node1_t30</t>
-  </si>
-  <si>
-    <t>Node1_t31</t>
-  </si>
-  <si>
-    <t>Node1_t32</t>
-  </si>
-  <si>
-    <t>Node1_t33</t>
-  </si>
-  <si>
-    <t>Node1_t34</t>
-  </si>
-  <si>
-    <t>Node1_t35</t>
-  </si>
-  <si>
-    <t>Node1_t36</t>
-  </si>
-  <si>
-    <t>Node1_t37</t>
-  </si>
-  <si>
-    <t>Node1_t38</t>
-  </si>
-  <si>
-    <t>Node1_t39</t>
-  </si>
-  <si>
-    <t>Node1_t40</t>
-  </si>
-  <si>
-    <t>Node1_t41</t>
-  </si>
-  <si>
-    <t>Node1_t42</t>
-  </si>
-  <si>
-    <t>Node2_t16</t>
-  </si>
-  <si>
-    <t>Node2_t17</t>
-  </si>
-  <si>
-    <t>Node2_t18</t>
-  </si>
-  <si>
-    <t>Node2_t19</t>
-  </si>
-  <si>
-    <t>Node2_t20</t>
-  </si>
-  <si>
-    <t>Node2_t21</t>
-  </si>
-  <si>
-    <t>Node2_t22</t>
-  </si>
-  <si>
-    <t>Node2_t23</t>
-  </si>
-  <si>
-    <t>Node2_t24</t>
-  </si>
-  <si>
-    <t>Node2_t25</t>
-  </si>
-  <si>
-    <t>Node2_t26</t>
-  </si>
-  <si>
-    <t>Node2_t27</t>
-  </si>
-  <si>
-    <t>Node2_t28</t>
-  </si>
-  <si>
-    <t>Node2_t29</t>
-  </si>
-  <si>
-    <t>Node2_t30</t>
-  </si>
-  <si>
-    <t>Node2_t31</t>
-  </si>
-  <si>
-    <t>Node2_t32</t>
-  </si>
-  <si>
-    <t>Node2_t33</t>
-  </si>
-  <si>
-    <t>Node2_t34</t>
-  </si>
-  <si>
-    <t>Node2_t35</t>
-  </si>
-  <si>
-    <t>Node2_t36</t>
-  </si>
-  <si>
-    <t>Node2_t37</t>
-  </si>
-  <si>
-    <t>Node2_t38</t>
-  </si>
-  <si>
-    <t>Node2_t39</t>
-  </si>
-  <si>
-    <t>Node2_t40</t>
-  </si>
-  <si>
-    <t>Node2_t41</t>
-  </si>
-  <si>
-    <t>Node2_t42</t>
-  </si>
-  <si>
-    <t>Node2_t43</t>
-  </si>
-  <si>
-    <t>Node2_t44</t>
-  </si>
-  <si>
-    <t>Node2_t45</t>
-  </si>
-  <si>
-    <t>Node2_t46</t>
-  </si>
-  <si>
-    <t>Node2_t47</t>
-  </si>
-  <si>
-    <t>Node2_t48</t>
-  </si>
-  <si>
-    <t>Node2_t49</t>
-  </si>
-  <si>
-    <t>Node2_t50</t>
-  </si>
-  <si>
-    <t>Node2_t51</t>
-  </si>
-  <si>
-    <t>Node2_t52</t>
-  </si>
-  <si>
-    <t>Node2_t53</t>
-  </si>
-  <si>
-    <t>Node2_t54</t>
-  </si>
-  <si>
-    <t>Node2_t55</t>
-  </si>
-  <si>
-    <t>Node2_t56</t>
-  </si>
-  <si>
-    <t>Node2_t57</t>
-  </si>
-  <si>
-    <t>Node2_t58</t>
-  </si>
-  <si>
-    <t>Node2_t59</t>
-  </si>
-  <si>
-    <t>Node3_t23</t>
-  </si>
-  <si>
-    <t>Node3_t24</t>
-  </si>
-  <si>
-    <t>Node3_t25</t>
-  </si>
-  <si>
-    <t>Node3_t26</t>
-  </si>
-  <si>
-    <t>Node3_t27</t>
-  </si>
-  <si>
-    <t>Node3_t28</t>
-  </si>
-  <si>
-    <t>Node3_t29</t>
-  </si>
-  <si>
-    <t>Node3_t30</t>
-  </si>
-  <si>
-    <t>Node3_t31</t>
-  </si>
-  <si>
-    <t>Node3_t32</t>
-  </si>
-  <si>
-    <t>Node3_t33</t>
-  </si>
-  <si>
-    <t>Node3_t34</t>
-  </si>
-  <si>
-    <t>Node3_t35</t>
-  </si>
-  <si>
-    <t>Node3_t36</t>
-  </si>
-  <si>
-    <t>Node3_t37</t>
-  </si>
-  <si>
-    <t>Node3_t38</t>
-  </si>
-  <si>
-    <t>Node3_t39</t>
-  </si>
-  <si>
-    <t>Node3_t40</t>
-  </si>
-  <si>
-    <t>Node3_t41</t>
-  </si>
-  <si>
-    <t>Node3_t42</t>
-  </si>
-  <si>
-    <t>Node3_t43</t>
-  </si>
-  <si>
-    <t>Node3_t44</t>
-  </si>
-  <si>
-    <t>Node3_t45</t>
-  </si>
-  <si>
-    <t>Node3_t64</t>
-  </si>
-  <si>
-    <t>Node3_t65</t>
-  </si>
-  <si>
-    <t>Node3_t66</t>
-  </si>
-  <si>
-    <t>Node3_t67</t>
-  </si>
-  <si>
-    <t>Node3_t68</t>
-  </si>
-  <si>
-    <t>Node3_t69</t>
-  </si>
-  <si>
-    <t>OD_Aarau_Chiasso_source</t>
-  </si>
-  <si>
-    <t>OD_Aarau_Visp_source</t>
-  </si>
-  <si>
-    <t>Node5_t22</t>
-  </si>
-  <si>
-    <t>OD_Baselwolf_Chiasso_source</t>
-  </si>
-  <si>
-    <t>Node3_t16</t>
-  </si>
-  <si>
-    <t>OD_Chiasso_Aarau_source</t>
   </si>
   <si>
     <t>Node1_t49</t>
@@ -1194,7 +1047,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I125"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1240,22 +1093,22 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="G2">
-        <v>80</v>
+        <v>29.4</v>
       </c>
       <c r="H2">
         <v>155.63758</v>
       </c>
       <c r="I2" t="s">
-        <v>260</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1269,22 +1122,22 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E3" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="F3" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="G3">
-        <v>0.8499999999999943</v>
+        <v>63</v>
       </c>
       <c r="H3">
-        <v>155.63758</v>
+        <v>151.515715</v>
       </c>
       <c r="I3" t="s">
-        <v>260</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1298,22 +1151,22 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>242</v>
+        <v>194</v>
       </c>
       <c r="F4" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="G4">
-        <v>63</v>
+        <v>52.9200000000003</v>
       </c>
       <c r="H4">
-        <v>151.515715</v>
+        <v>157.7173901587302</v>
       </c>
       <c r="I4" t="s">
-        <v>261</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1327,22 +1180,22 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="E5" t="s">
-        <v>244</v>
+        <v>184</v>
       </c>
       <c r="F5" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="G5">
-        <v>70.5600000000007</v>
+        <v>8</v>
       </c>
       <c r="H5">
         <v>157.7173901587302</v>
       </c>
       <c r="I5" t="s">
-        <v>262</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1356,22 +1209,22 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>234</v>
+        <v>196</v>
       </c>
       <c r="F6" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="H6">
-        <v>157.7173901587302</v>
+        <v>155.47652625</v>
       </c>
       <c r="I6" t="s">
-        <v>262</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1385,22 +1238,22 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
+        <v>197</v>
       </c>
       <c r="F7" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="G7">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="H7">
         <v>155.47652625</v>
       </c>
       <c r="I7" t="s">
-        <v>263</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1414,22 +1267,22 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="E8" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="F8" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="G8">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H8">
         <v>155.47652625</v>
       </c>
       <c r="I8" t="s">
-        <v>263</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1443,22 +1296,22 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="E9" t="s">
-        <v>247</v>
+        <v>117</v>
       </c>
       <c r="F9" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>51.26000000000022</v>
       </c>
       <c r="H9">
-        <v>155.47652625</v>
+        <v>157.6675138592233</v>
       </c>
       <c r="I9" t="s">
-        <v>263</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1472,22 +1325,22 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="E10" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="F10" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="G10">
-        <v>65.68000000000001</v>
+        <v>49</v>
       </c>
       <c r="H10">
-        <v>157.6675138592233</v>
+        <v>152.065055</v>
       </c>
       <c r="I10" t="s">
-        <v>264</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1501,22 +1354,19 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="F11" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="G11">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="H11">
-        <v>152.065055</v>
-      </c>
-      <c r="I11" t="s">
-        <v>265</v>
+        <v>1.333333333333333</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1530,16 +1380,16 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="F12" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G12">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H12">
         <v>1.333333333333333</v>
@@ -1556,16 +1406,16 @@
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="F13" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G13">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H13">
         <v>1.333333333333333</v>
@@ -1582,16 +1432,16 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="F14" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G14">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H14">
         <v>1.333333333333333</v>
@@ -1608,16 +1458,16 @@
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="F15" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G15">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H15">
         <v>1.333333333333333</v>
@@ -1634,16 +1484,16 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="E16" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F16" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G16">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H16">
         <v>1.333333333333333</v>
@@ -1660,16 +1510,16 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="E17" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="F17" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G17">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H17">
         <v>1.333333333333333</v>
@@ -1686,16 +1536,16 @@
         <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="E18" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="F18" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G18">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H18">
         <v>1.333333333333333</v>
@@ -1712,16 +1562,16 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="E19" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="F19" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G19">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H19">
         <v>1.333333333333333</v>
@@ -1738,16 +1588,16 @@
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="F20" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G20">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H20">
         <v>1.333333333333333</v>
@@ -1764,16 +1614,16 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="E21" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="F21" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G21">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H21">
         <v>1.333333333333333</v>
@@ -1790,16 +1640,16 @@
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="E22" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="F22" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G22">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H22">
         <v>1.333333333333333</v>
@@ -1816,16 +1666,16 @@
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="E23" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="F23" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G23">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H23">
         <v>1.333333333333333</v>
@@ -1842,16 +1692,16 @@
         <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="E24" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="F24" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G24">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H24">
         <v>1.333333333333333</v>
@@ -1868,16 +1718,16 @@
         <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="E25" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="F25" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G25">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H25">
         <v>1.333333333333333</v>
@@ -1894,16 +1744,16 @@
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="E26" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="F26" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G26">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H26">
         <v>1.333333333333333</v>
@@ -1920,16 +1770,16 @@
         <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="E27" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="F27" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G27">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H27">
         <v>1.333333333333333</v>
@@ -1946,16 +1796,16 @@
         <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="E28" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="F28" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G28">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H28">
         <v>1.333333333333333</v>
@@ -1972,16 +1822,16 @@
         <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="E29" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="F29" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G29">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H29">
         <v>1.333333333333333</v>
@@ -1998,16 +1848,16 @@
         <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="E30" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="F30" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G30">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H30">
         <v>1.333333333333333</v>
@@ -2024,16 +1874,16 @@
         <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="E31" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="F31" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G31">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H31">
         <v>1.333333333333333</v>
@@ -2050,16 +1900,16 @@
         <v>40</v>
       </c>
       <c r="D32" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="E32" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="F32" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G32">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H32">
         <v>1.333333333333333</v>
@@ -2076,16 +1926,16 @@
         <v>41</v>
       </c>
       <c r="D33" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="E33" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="F33" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G33">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H33">
         <v>1.333333333333333</v>
@@ -2102,16 +1952,16 @@
         <v>42</v>
       </c>
       <c r="D34" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="E34" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="F34" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G34">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H34">
         <v>1.333333333333333</v>
@@ -2128,16 +1978,16 @@
         <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="E35" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="F35" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G35">
-        <v>0.8499999999999943</v>
+        <v>8</v>
       </c>
       <c r="H35">
         <v>1.333333333333333</v>
@@ -2154,13 +2004,13 @@
         <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="E36" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="F36" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G36">
         <v>8</v>
@@ -2180,13 +2030,13 @@
         <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="E37" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="F37" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G37">
         <v>8</v>
@@ -2206,13 +2056,13 @@
         <v>46</v>
       </c>
       <c r="D38" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="E38" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="F38" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G38">
         <v>8</v>
@@ -2232,13 +2082,13 @@
         <v>47</v>
       </c>
       <c r="D39" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="E39" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="F39" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G39">
         <v>8</v>
@@ -2258,13 +2108,13 @@
         <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="E40" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="F40" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G40">
         <v>8</v>
@@ -2284,13 +2134,13 @@
         <v>49</v>
       </c>
       <c r="D41" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="E41" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="F41" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G41">
         <v>8</v>
@@ -2310,13 +2160,13 @@
         <v>50</v>
       </c>
       <c r="D42" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="E42" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="F42" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G42">
         <v>8</v>
@@ -2336,13 +2186,13 @@
         <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E43" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="F43" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G43">
         <v>8</v>
@@ -2362,13 +2212,13 @@
         <v>52</v>
       </c>
       <c r="D44" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="E44" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="F44" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G44">
         <v>8</v>
@@ -2388,13 +2238,13 @@
         <v>53</v>
       </c>
       <c r="D45" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="E45" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="F45" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G45">
         <v>8</v>
@@ -2414,13 +2264,13 @@
         <v>54</v>
       </c>
       <c r="D46" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="E46" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="F46" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G46">
         <v>8</v>
@@ -2440,13 +2290,13 @@
         <v>55</v>
       </c>
       <c r="D47" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="E47" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="F47" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G47">
         <v>8</v>
@@ -2466,13 +2316,13 @@
         <v>56</v>
       </c>
       <c r="D48" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="E48" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="F48" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G48">
         <v>8</v>
@@ -2492,13 +2342,13 @@
         <v>57</v>
       </c>
       <c r="D49" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="E49" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="F49" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G49">
         <v>8</v>
@@ -2518,13 +2368,13 @@
         <v>58</v>
       </c>
       <c r="D50" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="E50" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="F50" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G50">
         <v>8</v>
@@ -2544,13 +2394,13 @@
         <v>59</v>
       </c>
       <c r="D51" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="E51" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="F51" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G51">
         <v>8</v>
@@ -2570,13 +2420,13 @@
         <v>60</v>
       </c>
       <c r="D52" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="E52" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="F52" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G52">
         <v>8</v>
@@ -2596,13 +2446,13 @@
         <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="E53" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="F53" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G53">
         <v>8</v>
@@ -2622,13 +2472,13 @@
         <v>62</v>
       </c>
       <c r="D54" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="E54" t="s">
-        <v>186</v>
+        <v>111</v>
       </c>
       <c r="F54" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G54">
         <v>8</v>
@@ -2648,16 +2498,16 @@
         <v>63</v>
       </c>
       <c r="D55" t="s">
-        <v>186</v>
+        <v>112</v>
       </c>
       <c r="E55" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="F55" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G55">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H55">
         <v>1.333333333333333</v>
@@ -2674,16 +2524,16 @@
         <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="E56" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="F56" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G56">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H56">
         <v>1.333333333333333</v>
@@ -2700,16 +2550,16 @@
         <v>65</v>
       </c>
       <c r="D57" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="E57" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="F57" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G57">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H57">
         <v>1.333333333333333</v>
@@ -2726,16 +2576,16 @@
         <v>66</v>
       </c>
       <c r="D58" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="E58" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="F58" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G58">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H58">
         <v>1.333333333333333</v>
@@ -2752,16 +2602,16 @@
         <v>67</v>
       </c>
       <c r="D59" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="E59" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="F59" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G59">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H59">
         <v>1.333333333333333</v>
@@ -2778,16 +2628,16 @@
         <v>68</v>
       </c>
       <c r="D60" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="E60" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="F60" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G60">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H60">
         <v>1.333333333333333</v>
@@ -2804,16 +2654,16 @@
         <v>69</v>
       </c>
       <c r="D61" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="E61" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="F61" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G61">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H61">
         <v>1.333333333333333</v>
@@ -2830,16 +2680,16 @@
         <v>70</v>
       </c>
       <c r="D62" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="E62" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="F62" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G62">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H62">
         <v>1.333333333333333</v>
@@ -2856,16 +2706,16 @@
         <v>71</v>
       </c>
       <c r="D63" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="E63" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="F63" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G63">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H63">
         <v>1.333333333333333</v>
@@ -2882,16 +2732,16 @@
         <v>72</v>
       </c>
       <c r="D64" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="E64" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="F64" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G64">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H64">
         <v>1.333333333333333</v>
@@ -2908,16 +2758,16 @@
         <v>73</v>
       </c>
       <c r="D65" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="E65" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="F65" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G65">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H65">
         <v>1.333333333333333</v>
@@ -2934,16 +2784,16 @@
         <v>74</v>
       </c>
       <c r="D66" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="E66" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="F66" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G66">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H66">
         <v>1.333333333333333</v>
@@ -2960,16 +2810,16 @@
         <v>75</v>
       </c>
       <c r="D67" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="E67" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="F67" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G67">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H67">
         <v>1.333333333333333</v>
@@ -2986,16 +2836,16 @@
         <v>76</v>
       </c>
       <c r="D68" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="E68" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="F68" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G68">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H68">
         <v>1.333333333333333</v>
@@ -3012,16 +2862,16 @@
         <v>77</v>
       </c>
       <c r="D69" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="E69" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="F69" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G69">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H69">
         <v>1.333333333333333</v>
@@ -3038,16 +2888,16 @@
         <v>78</v>
       </c>
       <c r="D70" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="E70" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="F70" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G70">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H70">
         <v>1.333333333333333</v>
@@ -3064,16 +2914,16 @@
         <v>79</v>
       </c>
       <c r="D71" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="E71" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="F71" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G71">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H71">
         <v>1.333333333333333</v>
@@ -3090,16 +2940,16 @@
         <v>80</v>
       </c>
       <c r="D72" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="E72" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="F72" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G72">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H72">
         <v>1.333333333333333</v>
@@ -3116,16 +2966,16 @@
         <v>81</v>
       </c>
       <c r="D73" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="E73" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="F73" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G73">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H73">
         <v>1.333333333333333</v>
@@ -3142,16 +2992,16 @@
         <v>82</v>
       </c>
       <c r="D74" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="E74" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="F74" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G74">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H74">
         <v>1.333333333333333</v>
@@ -3168,16 +3018,16 @@
         <v>83</v>
       </c>
       <c r="D75" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="E75" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="F75" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G75">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H75">
         <v>1.333333333333333</v>
@@ -3194,16 +3044,16 @@
         <v>84</v>
       </c>
       <c r="D76" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="E76" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="F76" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G76">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H76">
         <v>1.333333333333333</v>
@@ -3220,16 +3070,16 @@
         <v>85</v>
       </c>
       <c r="D77" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="E77" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="F77" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G77">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H77">
         <v>1.333333333333333</v>
@@ -3246,16 +3096,16 @@
         <v>86</v>
       </c>
       <c r="D78" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="E78" t="s">
-        <v>210</v>
+        <v>113</v>
       </c>
       <c r="F78" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G78">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H78">
         <v>1.333333333333333</v>
@@ -3272,13 +3122,13 @@
         <v>87</v>
       </c>
       <c r="D79" t="s">
-        <v>210</v>
+        <v>184</v>
       </c>
       <c r="E79" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="F79" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G79">
         <v>8</v>
@@ -3298,22 +3148,22 @@
         <v>88</v>
       </c>
       <c r="D80" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="E80" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="F80" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G80">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H80">
         <v>1.333333333333333</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -3324,22 +3174,22 @@
         <v>89</v>
       </c>
       <c r="D81" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="E81" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="F81" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G81">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H81">
         <v>1.333333333333333</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>9</v>
       </c>
@@ -3350,22 +3200,22 @@
         <v>90</v>
       </c>
       <c r="D82" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="E82" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="F82" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G82">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H82">
         <v>1.333333333333333</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -3376,22 +3226,22 @@
         <v>91</v>
       </c>
       <c r="D83" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="E83" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="F83" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G83">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H83">
         <v>1.333333333333333</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>9</v>
       </c>
@@ -3402,22 +3252,22 @@
         <v>92</v>
       </c>
       <c r="D84" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="E84" t="s">
-        <v>215</v>
+        <v>114</v>
       </c>
       <c r="F84" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="G84">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H84">
         <v>1.333333333333333</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>9</v>
       </c>
@@ -3428,22 +3278,25 @@
         <v>93</v>
       </c>
       <c r="D85" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="E85" t="s">
-        <v>216</v>
+        <v>108</v>
       </c>
       <c r="F85" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
       <c r="G85">
-        <v>24</v>
+        <v>29.4</v>
       </c>
       <c r="H85">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I85" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>9</v>
       </c>
@@ -3454,22 +3307,25 @@
         <v>94</v>
       </c>
       <c r="D86" t="s">
-        <v>216</v>
+        <v>112</v>
       </c>
       <c r="E86" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="F86" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="G86">
-        <v>24</v>
+        <v>29.4</v>
       </c>
       <c r="H86">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I86" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -3480,22 +3336,25 @@
         <v>95</v>
       </c>
       <c r="D87" t="s">
-        <v>217</v>
+        <v>191</v>
       </c>
       <c r="E87" t="s">
-        <v>218</v>
+        <v>109</v>
       </c>
       <c r="F87" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
       <c r="G87">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="H87">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I87" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>9</v>
       </c>
@@ -3506,22 +3365,25 @@
         <v>96</v>
       </c>
       <c r="D88" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="E88" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="F88" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="G88">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="H88">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I88" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>9</v>
       </c>
@@ -3532,22 +3394,25 @@
         <v>97</v>
       </c>
       <c r="D89" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="E89" t="s">
-        <v>220</v>
+        <v>110</v>
       </c>
       <c r="F89" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
       <c r="G89">
-        <v>24</v>
+        <v>52.9200000000003</v>
       </c>
       <c r="H89">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I89" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>9</v>
       </c>
@@ -3558,22 +3423,25 @@
         <v>98</v>
       </c>
       <c r="D90" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="E90" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="F90" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="G90">
-        <v>24</v>
+        <v>52.9200000000003</v>
       </c>
       <c r="H90">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I90" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>9</v>
       </c>
@@ -3584,22 +3452,25 @@
         <v>99</v>
       </c>
       <c r="D91" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="E91" t="s">
-        <v>222</v>
+        <v>115</v>
       </c>
       <c r="F91" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
       <c r="G91">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H91">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I91" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>9</v>
       </c>
@@ -3610,22 +3481,25 @@
         <v>100</v>
       </c>
       <c r="D92" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="E92" t="s">
-        <v>223</v>
+        <v>112</v>
       </c>
       <c r="F92" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
       <c r="G92">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="H92">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I92" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -3636,22 +3510,25 @@
         <v>101</v>
       </c>
       <c r="D93" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="E93" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="F93" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="G93">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="H93">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I93" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -3662,22 +3539,25 @@
         <v>102</v>
       </c>
       <c r="D94" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="E94" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="F94" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="G94">
         <v>24</v>
       </c>
       <c r="H94">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I94" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -3688,22 +3568,25 @@
         <v>103</v>
       </c>
       <c r="D95" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="E95" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
       <c r="F95" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="G95">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H95">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>9</v>
       </c>
@@ -3714,19 +3597,22 @@
         <v>104</v>
       </c>
       <c r="D96" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
       <c r="E96" t="s">
-        <v>227</v>
+        <v>115</v>
       </c>
       <c r="F96" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
       <c r="G96">
-        <v>24</v>
+        <v>43.26000000000022</v>
       </c>
       <c r="H96">
-        <v>1.333333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="I96" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3740,19 +3626,22 @@
         <v>105</v>
       </c>
       <c r="D97" t="s">
-        <v>227</v>
+        <v>117</v>
       </c>
       <c r="E97" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="F97" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="G97">
-        <v>24</v>
+        <v>43.26000000000022</v>
       </c>
       <c r="H97">
-        <v>1.333333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="I97" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3766,19 +3655,22 @@
         <v>106</v>
       </c>
       <c r="D98" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
       <c r="E98" t="s">
-        <v>229</v>
+        <v>116</v>
       </c>
       <c r="F98" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
       <c r="G98">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="H98">
-        <v>1.333333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="I98" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3792,743 +3684,22 @@
         <v>107</v>
       </c>
       <c r="D99" t="s">
-        <v>229</v>
+        <v>109</v>
       </c>
       <c r="E99" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="F99" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="G99">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="H99">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100" t="s">
-        <v>9</v>
-      </c>
-      <c r="B100" t="s">
-        <v>9</v>
-      </c>
-      <c r="C100" t="s">
-        <v>108</v>
-      </c>
-      <c r="D100" t="s">
-        <v>230</v>
-      </c>
-      <c r="E100" t="s">
-        <v>231</v>
-      </c>
-      <c r="F100" t="s">
-        <v>257</v>
-      </c>
-      <c r="G100">
-        <v>24</v>
-      </c>
-      <c r="H100">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
-      <c r="A101" t="s">
-        <v>9</v>
-      </c>
-      <c r="B101" t="s">
-        <v>9</v>
-      </c>
-      <c r="C101" t="s">
-        <v>109</v>
-      </c>
-      <c r="D101" t="s">
-        <v>231</v>
-      </c>
-      <c r="E101" t="s">
-        <v>232</v>
-      </c>
-      <c r="F101" t="s">
-        <v>257</v>
-      </c>
-      <c r="G101">
-        <v>24</v>
-      </c>
-      <c r="H101">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
-      <c r="A102" t="s">
-        <v>9</v>
-      </c>
-      <c r="B102" t="s">
-        <v>9</v>
-      </c>
-      <c r="C102" t="s">
-        <v>110</v>
-      </c>
-      <c r="D102" t="s">
-        <v>232</v>
-      </c>
-      <c r="E102" t="s">
-        <v>233</v>
-      </c>
-      <c r="F102" t="s">
-        <v>257</v>
-      </c>
-      <c r="G102">
-        <v>24</v>
-      </c>
-      <c r="H102">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
-      <c r="A103" t="s">
-        <v>9</v>
-      </c>
-      <c r="B103" t="s">
-        <v>9</v>
-      </c>
-      <c r="C103" t="s">
-        <v>111</v>
-      </c>
-      <c r="D103" t="s">
-        <v>233</v>
-      </c>
-      <c r="E103" t="s">
-        <v>140</v>
-      </c>
-      <c r="F103" t="s">
-        <v>257</v>
-      </c>
-      <c r="G103">
-        <v>24</v>
-      </c>
-      <c r="H103">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
-      <c r="A104" t="s">
-        <v>9</v>
-      </c>
-      <c r="B104" t="s">
-        <v>9</v>
-      </c>
-      <c r="C104" t="s">
-        <v>112</v>
-      </c>
-      <c r="D104" t="s">
-        <v>234</v>
-      </c>
-      <c r="E104" t="s">
-        <v>235</v>
-      </c>
-      <c r="F104" t="s">
-        <v>257</v>
-      </c>
-      <c r="G104">
-        <v>8</v>
-      </c>
-      <c r="H104">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
-      <c r="A105" t="s">
-        <v>9</v>
-      </c>
-      <c r="B105" t="s">
-        <v>9</v>
-      </c>
-      <c r="C105" t="s">
-        <v>113</v>
-      </c>
-      <c r="D105" t="s">
-        <v>235</v>
-      </c>
-      <c r="E105" t="s">
-        <v>236</v>
-      </c>
-      <c r="F105" t="s">
-        <v>257</v>
-      </c>
-      <c r="G105">
-        <v>8</v>
-      </c>
-      <c r="H105">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
-      <c r="A106" t="s">
-        <v>9</v>
-      </c>
-      <c r="B106" t="s">
-        <v>9</v>
-      </c>
-      <c r="C106" t="s">
-        <v>114</v>
-      </c>
-      <c r="D106" t="s">
-        <v>236</v>
-      </c>
-      <c r="E106" t="s">
-        <v>237</v>
-      </c>
-      <c r="F106" t="s">
-        <v>257</v>
-      </c>
-      <c r="G106">
-        <v>8</v>
-      </c>
-      <c r="H106">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
-      <c r="A107" t="s">
-        <v>9</v>
-      </c>
-      <c r="B107" t="s">
-        <v>9</v>
-      </c>
-      <c r="C107" t="s">
-        <v>115</v>
-      </c>
-      <c r="D107" t="s">
-        <v>237</v>
-      </c>
-      <c r="E107" t="s">
-        <v>238</v>
-      </c>
-      <c r="F107" t="s">
-        <v>257</v>
-      </c>
-      <c r="G107">
-        <v>8</v>
-      </c>
-      <c r="H107">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
-      <c r="A108" t="s">
-        <v>9</v>
-      </c>
-      <c r="B108" t="s">
-        <v>9</v>
-      </c>
-      <c r="C108" t="s">
-        <v>116</v>
-      </c>
-      <c r="D108" t="s">
-        <v>238</v>
-      </c>
-      <c r="E108" t="s">
-        <v>239</v>
-      </c>
-      <c r="F108" t="s">
-        <v>257</v>
-      </c>
-      <c r="G108">
-        <v>8</v>
-      </c>
-      <c r="H108">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9">
-      <c r="A109" t="s">
-        <v>9</v>
-      </c>
-      <c r="B109" t="s">
-        <v>9</v>
-      </c>
-      <c r="C109" t="s">
-        <v>117</v>
-      </c>
-      <c r="D109" t="s">
-        <v>239</v>
-      </c>
-      <c r="E109" t="s">
-        <v>141</v>
-      </c>
-      <c r="F109" t="s">
-        <v>257</v>
-      </c>
-      <c r="G109">
-        <v>8</v>
-      </c>
-      <c r="H109">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9">
-      <c r="A110" t="s">
-        <v>9</v>
-      </c>
-      <c r="B110" t="s">
-        <v>9</v>
-      </c>
-      <c r="C110" t="s">
-        <v>118</v>
-      </c>
-      <c r="D110" t="s">
-        <v>240</v>
-      </c>
-      <c r="E110" t="s">
-        <v>134</v>
-      </c>
-      <c r="F110" t="s">
-        <v>258</v>
-      </c>
-      <c r="G110">
-        <v>80.84999999999999</v>
-      </c>
-      <c r="H110">
         <v>0</v>
       </c>
-      <c r="I110" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9">
-      <c r="A111" t="s">
-        <v>9</v>
-      </c>
-      <c r="B111" t="s">
-        <v>9</v>
-      </c>
-      <c r="C111" t="s">
-        <v>119</v>
-      </c>
-      <c r="D111" t="s">
-        <v>139</v>
-      </c>
-      <c r="E111" t="s">
-        <v>250</v>
-      </c>
-      <c r="F111" t="s">
-        <v>259</v>
-      </c>
-      <c r="G111">
-        <v>80</v>
-      </c>
-      <c r="H111">
-        <v>0</v>
-      </c>
-      <c r="I111" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9">
-      <c r="A112" t="s">
-        <v>9</v>
-      </c>
-      <c r="B112" t="s">
-        <v>9</v>
-      </c>
-      <c r="C112" t="s">
-        <v>120</v>
-      </c>
-      <c r="D112" t="s">
-        <v>140</v>
-      </c>
-      <c r="E112" t="s">
-        <v>250</v>
-      </c>
-      <c r="F112" t="s">
-        <v>259</v>
-      </c>
-      <c r="G112">
-        <v>0.8499999999999943</v>
-      </c>
-      <c r="H112">
-        <v>0</v>
-      </c>
-      <c r="I112" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
-      <c r="A113" t="s">
-        <v>9</v>
-      </c>
-      <c r="B113" t="s">
-        <v>9</v>
-      </c>
-      <c r="C113" t="s">
-        <v>121</v>
-      </c>
-      <c r="D113" t="s">
-        <v>241</v>
-      </c>
-      <c r="E113" t="s">
-        <v>136</v>
-      </c>
-      <c r="F113" t="s">
-        <v>258</v>
-      </c>
-      <c r="G113">
-        <v>63</v>
-      </c>
-      <c r="H113">
-        <v>0</v>
-      </c>
-      <c r="I113" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9">
-      <c r="A114" t="s">
-        <v>9</v>
-      </c>
-      <c r="B114" t="s">
-        <v>9</v>
-      </c>
-      <c r="C114" t="s">
-        <v>122</v>
-      </c>
-      <c r="D114" t="s">
-        <v>242</v>
-      </c>
-      <c r="E114" t="s">
-        <v>251</v>
-      </c>
-      <c r="F114" t="s">
-        <v>259</v>
-      </c>
-      <c r="G114">
-        <v>63</v>
-      </c>
-      <c r="H114">
-        <v>0</v>
-      </c>
-      <c r="I114" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9">
-      <c r="A115" t="s">
-        <v>9</v>
-      </c>
-      <c r="B115" t="s">
-        <v>9</v>
-      </c>
-      <c r="C115" t="s">
-        <v>123</v>
-      </c>
-      <c r="D115" t="s">
-        <v>243</v>
-      </c>
-      <c r="E115" t="s">
-        <v>137</v>
-      </c>
-      <c r="F115" t="s">
-        <v>258</v>
-      </c>
-      <c r="G115">
-        <v>70.5600000000007</v>
-      </c>
-      <c r="H115">
-        <v>0</v>
-      </c>
-      <c r="I115" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
-      <c r="A116" t="s">
-        <v>9</v>
-      </c>
-      <c r="B116" t="s">
-        <v>9</v>
-      </c>
-      <c r="C116" t="s">
-        <v>124</v>
-      </c>
-      <c r="D116" t="s">
-        <v>244</v>
-      </c>
-      <c r="E116" t="s">
-        <v>252</v>
-      </c>
-      <c r="F116" t="s">
-        <v>259</v>
-      </c>
-      <c r="G116">
-        <v>70.5600000000007</v>
-      </c>
-      <c r="H116">
-        <v>0</v>
-      </c>
-      <c r="I116" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9">
-      <c r="A117" t="s">
-        <v>9</v>
-      </c>
-      <c r="B117" t="s">
-        <v>9</v>
-      </c>
-      <c r="C117" t="s">
-        <v>125</v>
-      </c>
-      <c r="D117" t="s">
-        <v>245</v>
-      </c>
-      <c r="E117" t="s">
-        <v>142</v>
-      </c>
-      <c r="F117" t="s">
-        <v>258</v>
-      </c>
-      <c r="G117">
-        <v>8</v>
-      </c>
-      <c r="H117">
-        <v>0</v>
-      </c>
-      <c r="I117" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9">
-      <c r="A118" t="s">
-        <v>9</v>
-      </c>
-      <c r="B118" t="s">
-        <v>9</v>
-      </c>
-      <c r="C118" t="s">
-        <v>126</v>
-      </c>
-      <c r="D118" t="s">
-        <v>245</v>
-      </c>
-      <c r="E118" t="s">
-        <v>139</v>
-      </c>
-      <c r="F118" t="s">
-        <v>258</v>
-      </c>
-      <c r="G118">
-        <v>104</v>
-      </c>
-      <c r="H118">
-        <v>0</v>
-      </c>
-      <c r="I118" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
-      <c r="A119" t="s">
-        <v>9</v>
-      </c>
-      <c r="B119" t="s">
-        <v>9</v>
-      </c>
-      <c r="C119" t="s">
-        <v>127</v>
-      </c>
-      <c r="D119" t="s">
-        <v>149</v>
-      </c>
-      <c r="E119" t="s">
-        <v>253</v>
-      </c>
-      <c r="F119" t="s">
-        <v>259</v>
-      </c>
-      <c r="G119">
-        <v>80</v>
-      </c>
-      <c r="H119">
-        <v>0</v>
-      </c>
-      <c r="I119" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
-      <c r="A120" t="s">
-        <v>9</v>
-      </c>
-      <c r="B120" t="s">
-        <v>9</v>
-      </c>
-      <c r="C120" t="s">
-        <v>128</v>
-      </c>
-      <c r="D120" t="s">
-        <v>246</v>
-      </c>
-      <c r="E120" t="s">
-        <v>253</v>
-      </c>
-      <c r="F120" t="s">
-        <v>259</v>
-      </c>
-      <c r="G120">
-        <v>24</v>
-      </c>
-      <c r="H120">
-        <v>0</v>
-      </c>
-      <c r="I120" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
-      <c r="A121" t="s">
-        <v>9</v>
-      </c>
-      <c r="B121" t="s">
-        <v>9</v>
-      </c>
-      <c r="C121" t="s">
-        <v>129</v>
-      </c>
-      <c r="D121" t="s">
-        <v>247</v>
-      </c>
-      <c r="E121" t="s">
-        <v>253</v>
-      </c>
-      <c r="F121" t="s">
-        <v>259</v>
-      </c>
-      <c r="G121">
-        <v>8</v>
-      </c>
-      <c r="H121">
-        <v>0</v>
-      </c>
-      <c r="I121" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
-      <c r="A122" t="s">
-        <v>9</v>
-      </c>
-      <c r="B122" t="s">
-        <v>9</v>
-      </c>
-      <c r="C122" t="s">
-        <v>130</v>
-      </c>
-      <c r="D122" t="s">
-        <v>248</v>
-      </c>
-      <c r="E122" t="s">
-        <v>142</v>
-      </c>
-      <c r="F122" t="s">
-        <v>258</v>
-      </c>
-      <c r="G122">
-        <v>57.68</v>
-      </c>
-      <c r="H122">
-        <v>0</v>
-      </c>
-      <c r="I122" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
-      <c r="A123" t="s">
-        <v>9</v>
-      </c>
-      <c r="B123" t="s">
-        <v>9</v>
-      </c>
-      <c r="C123" t="s">
-        <v>131</v>
-      </c>
-      <c r="D123" t="s">
-        <v>167</v>
-      </c>
-      <c r="E123" t="s">
-        <v>254</v>
-      </c>
-      <c r="F123" t="s">
-        <v>259</v>
-      </c>
-      <c r="G123">
-        <v>57.68</v>
-      </c>
-      <c r="H123">
-        <v>0</v>
-      </c>
-      <c r="I123" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
-      <c r="A124" t="s">
-        <v>9</v>
-      </c>
-      <c r="B124" t="s">
-        <v>9</v>
-      </c>
-      <c r="C124" t="s">
-        <v>132</v>
-      </c>
-      <c r="D124" t="s">
-        <v>249</v>
-      </c>
-      <c r="E124" t="s">
-        <v>143</v>
-      </c>
-      <c r="F124" t="s">
-        <v>258</v>
-      </c>
-      <c r="G124">
-        <v>49</v>
-      </c>
-      <c r="H124">
-        <v>0</v>
-      </c>
-      <c r="I124" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
-      <c r="A125" t="s">
-        <v>9</v>
-      </c>
-      <c r="B125" t="s">
-        <v>9</v>
-      </c>
-      <c r="C125" t="s">
-        <v>133</v>
-      </c>
-      <c r="D125" t="s">
-        <v>136</v>
-      </c>
-      <c r="E125" t="s">
-        <v>255</v>
-      </c>
-      <c r="F125" t="s">
-        <v>259</v>
-      </c>
-      <c r="G125">
-        <v>49</v>
-      </c>
-      <c r="H125">
-        <v>0</v>
-      </c>
-      <c r="I125" t="s">
-        <v>265</v>
+      <c r="I99" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -4552,16 +3723,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>266</v>
+        <v>217</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>267</v>
+        <v>218</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>8</v>
@@ -4569,33 +3740,33 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>222</v>
       </c>
       <c r="C2">
-        <v>80.84999999999999</v>
+        <v>29.4</v>
       </c>
       <c r="D2">
-        <v>80.84999999999999</v>
+        <v>29.4</v>
       </c>
       <c r="E2">
-        <v>80.85000000000002</v>
+        <v>154.35</v>
       </c>
       <c r="F2">
-        <v>99.99999999999997</v>
+        <v>19.04761904761905</v>
       </c>
       <c r="G2" t="s">
-        <v>260</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
       <c r="C3">
         <v>112</v>
@@ -4610,15 +3781,15 @@
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>263</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>223</v>
       </c>
       <c r="C4">
         <v>63</v>
@@ -4633,15 +3804,15 @@
         <v>78.75</v>
       </c>
       <c r="G4" t="s">
-        <v>261</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
       <c r="C5">
         <v>49</v>
@@ -4656,53 +3827,53 @@
         <v>61.25000000000001</v>
       </c>
       <c r="G5" t="s">
-        <v>265</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>224</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>222</v>
       </c>
       <c r="C6">
-        <v>70.5600000000007</v>
+        <v>52.9200000000003</v>
       </c>
       <c r="D6">
-        <v>70.5600000000007</v>
+        <v>52.9200000000003</v>
       </c>
       <c r="E6">
         <v>80</v>
       </c>
       <c r="F6">
-        <v>88.20000000000088</v>
+        <v>66.15000000000038</v>
       </c>
       <c r="G6" t="s">
-        <v>262</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>271</v>
+        <v>222</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>224</v>
       </c>
       <c r="C7">
-        <v>57.68</v>
+        <v>43.26000000000022</v>
       </c>
       <c r="D7">
-        <v>57.68</v>
+        <v>43.26000000000022</v>
       </c>
       <c r="E7">
-        <v>80</v>
+        <v>121.1280000000007</v>
       </c>
       <c r="F7">
-        <v>72.09999999999999</v>
+        <v>35.71428571428569</v>
       </c>
       <c r="G7" t="s">
-        <v>264</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>